<commit_message>
refactor(audio): Refactor taunt logic, update enemy names, and improve activity taunt tracking (v0.5.0)
This commit refactors the taunt logic for better maintainability, updates enemy names in taunt clips, and improves activity taunt tracking.

The following changes were made:

- **Refactoring:**
    - Broke down the `Taunt` method into smaller, more manageable methods for improved readability and maintainability.
- **Enemy Name Updates:**
    - Changed some enemy names in taunt clips to align with internal enemy names, ensuring consistency.
- **Activity Taunt Tracking:**
    - Removed the expiration timer for activity taunts.
    - Added player-specific timers for each activity type to prevent repeated taunts within 60 seconds.
- **Default Taunts:**
    - Added an additional default Steam ID taunt to ensure the array loads correctly.

These changes enhance the organization, accuracy, and behavior of the gargoyle's taunt system.
</commit_message>
<xml_diff>
--- a/AssetSources/Audio/VoiceLines.xlsx
+++ b/AssetSources/Audio/VoiceLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753AA1FF-6C68-4D1E-9917-E1ACF28D7719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F6763-6314-4A2E-A23B-C5B22BFC094B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28200" yWindow="975" windowWidth="29010" windowHeight="15345" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="-28800" yWindow="660" windowWidth="29010" windowHeight="15345" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Taunts" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="343">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -978,12 +978,6 @@
     <t>Centipede</t>
   </si>
   <si>
-    <t>GhostGirl</t>
-  </si>
-  <si>
-    <t>HoardingBug</t>
-  </si>
-  <si>
     <t>Jester</t>
   </si>
   <si>
@@ -996,30 +990,9 @@
     <t>Nutcracker</t>
   </si>
   <si>
-    <t>Slime</t>
-  </si>
-  <si>
-    <t>Spider</t>
-  </si>
-  <si>
-    <t>SpringHead</t>
-  </si>
-  <si>
-    <t>Thumper</t>
-  </si>
-  <si>
-    <t>Action_Pickup</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
-    <t>Action_KilledEnemy</t>
-  </si>
-  <si>
-    <t>Action_FacilityTime</t>
-  </si>
-  <si>
     <t>Apparatus</t>
   </si>
   <si>
@@ -1099,6 +1072,45 @@
   </si>
   <si>
     <t>"Oh, look at me! I'm an employee, I'm so strong that I kill toys! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>Activity_Pickup</t>
+  </si>
+  <si>
+    <t>Activity_KilledEnemy</t>
+  </si>
+  <si>
+    <t>Activity_FacilityTime</t>
+  </si>
+  <si>
+    <t>Crawler</t>
+  </si>
+  <si>
+    <t>Girl</t>
+  </si>
+  <si>
+    <t>Flowerman</t>
+  </si>
+  <si>
+    <t>Blob</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Bunker Spider</t>
+  </si>
+  <si>
+    <t>Hoarding Bug</t>
+  </si>
+  <si>
+    <t>"If it isn't my creator! There's something I've always wanted to say to you, YOU SUCK! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>76561198155447311</t>
+  </si>
+  <si>
+    <t>MyCreator</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1170,11 +1182,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1196,15 +1227,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1251,8 +1273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H166" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:H166" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H167" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H167" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H139">
     <sortCondition ref="G1:G139"/>
   </sortState>
@@ -1260,13 +1282,13 @@
     <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{6266219D-B50E-4703-B88B-14976C41CFC3}" name="Redo" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="6">
       <calculatedColumnFormula>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="5">
       <calculatedColumnFormula>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1591,11 +1613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H167" sqref="H167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1626,7 @@
     <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="89.42578125" customWidth="1"/>
@@ -1623,7 +1645,7 @@
       <c r="D1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1646,15 +1668,15 @@
       <c r="D2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>308</v>
+      <c r="E2" s="8" t="s">
+        <v>330</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G2" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F2</f>
-        <v>taunt_action_pickup_Maneater</v>
+        <v>taunt_activity_pickup_Maneater</v>
       </c>
       <c r="H2" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -1671,7 +1693,7 @@
       <c r="D3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1696,7 +1718,7 @@
       <c r="D4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1721,7 +1743,7 @@
       <c r="D5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1746,7 +1768,7 @@
       <c r="D6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1771,7 +1793,7 @@
       <c r="D7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1793,7 +1815,7 @@
       <c r="D8" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1818,7 +1840,7 @@
       <c r="D9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1843,7 +1865,7 @@
       <c r="D10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1868,7 +1890,7 @@
       <c r="D11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1893,15 +1915,15 @@
       <c r="D12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>61</v>
+        <v>335</v>
       </c>
       <c r="G12" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F12</f>
-        <v>taunt_enemy_Bracken</v>
+        <v>taunt_enemy_Flowerman</v>
       </c>
       <c r="H12" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -1918,7 +1940,7 @@
       <c r="D13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1943,7 +1965,7 @@
       <c r="D14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1968,15 +1990,15 @@
       <c r="D15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="G15" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F15</f>
-        <v>taunt_enemy_GhostGirl</v>
+        <v>taunt_enemy_Girl</v>
       </c>
       <c r="H15" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -1993,15 +2015,15 @@
       <c r="D16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
       <c r="G16" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F16</f>
-        <v>taunt_enemy_HoardingBug</v>
+        <v>taunt_enemy_Hoarding Bug</v>
       </c>
       <c r="H16" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -2018,11 +2040,11 @@
       <c r="D17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G17" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F17</f>
@@ -2043,11 +2065,11 @@
       <c r="D18" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G18" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F18</f>
@@ -2068,11 +2090,11 @@
       <c r="D19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G19" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F19</f>
@@ -2093,11 +2115,11 @@
       <c r="D20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G20" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F20</f>
@@ -2118,15 +2140,15 @@
       <c r="D21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="G21" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F21</f>
-        <v>taunt_enemy_Slime</v>
+        <v>taunt_enemy_Blob</v>
       </c>
       <c r="H21" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -2143,15 +2165,15 @@
       <c r="D22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="G22" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F22</f>
-        <v>taunt_enemy_Spider</v>
+        <v>taunt_enemy_Bunker Spider</v>
       </c>
       <c r="H22" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -2168,15 +2190,15 @@
       <c r="D23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="G23" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F23</f>
-        <v>taunt_enemy_SpringHead</v>
+        <v>taunt_enemy_Spring</v>
       </c>
       <c r="H23" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -2193,15 +2215,15 @@
       <c r="D24" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="G24" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F24</f>
-        <v>taunt_enemy_Thumper</v>
+        <v>taunt_enemy_Crawler</v>
       </c>
       <c r="H24" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -2218,7 +2240,7 @@
       <c r="D25" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2243,7 +2265,7 @@
       <c r="D26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -2268,7 +2290,7 @@
       <c r="D27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -2293,7 +2315,7 @@
       <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -2318,7 +2340,7 @@
       <c r="D29" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -2343,7 +2365,7 @@
       <c r="D30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F30" s="4" t="s">
@@ -2368,7 +2390,7 @@
       <c r="D31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -2393,7 +2415,7 @@
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -2418,7 +2440,7 @@
       <c r="D33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F33" s="4" t="s">
@@ -2443,7 +2465,7 @@
       <c r="D34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F34" s="4" t="s">
@@ -2468,7 +2490,7 @@
       <c r="D35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -2493,7 +2515,7 @@
       <c r="D36" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -2518,7 +2540,7 @@
       <c r="D37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F37" s="4" t="s">
@@ -2543,7 +2565,7 @@
       <c r="D38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -2568,7 +2590,7 @@
       <c r="D39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -2593,7 +2615,7 @@
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -2618,7 +2640,7 @@
       <c r="D41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F41" s="4" t="s">
@@ -2643,7 +2665,7 @@
       <c r="D42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F42" s="4" t="s">
@@ -2668,7 +2690,7 @@
       <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -2693,7 +2715,7 @@
       <c r="D44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -2718,7 +2740,7 @@
       <c r="D45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F45" s="4" t="s">
@@ -2743,7 +2765,7 @@
       <c r="D46" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F46" s="4" t="s">
@@ -2768,7 +2790,7 @@
       <c r="D47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -2793,7 +2815,7 @@
       <c r="D48" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -2818,7 +2840,7 @@
       <c r="D49" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F49" s="4" t="s">
@@ -2843,7 +2865,7 @@
       <c r="D50" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F50" s="4" t="s">
@@ -2868,7 +2890,7 @@
       <c r="D51" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F51" s="4" t="s">
@@ -2893,7 +2915,7 @@
       <c r="D52" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F52" s="4" t="s">
@@ -2918,7 +2940,7 @@
       <c r="D53" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F53" s="4" t="s">
@@ -2943,7 +2965,7 @@
       <c r="D54" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F54" s="4" t="s">
@@ -2968,7 +2990,7 @@
       <c r="D55" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F55" s="4" t="s">
@@ -2993,7 +3015,7 @@
       <c r="D56" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -3018,7 +3040,7 @@
       <c r="D57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -3043,7 +3065,7 @@
       <c r="D58" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F58" s="4" t="s">
@@ -3068,7 +3090,7 @@
       <c r="D59" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F59" s="4" t="s">
@@ -3093,7 +3115,7 @@
       <c r="D60" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F60" s="4" t="s">
@@ -3118,7 +3140,7 @@
       <c r="D61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -3143,7 +3165,7 @@
       <c r="D62" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -3168,7 +3190,7 @@
       <c r="D63" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F63" s="4" t="s">
@@ -3193,7 +3215,7 @@
       <c r="D64" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -3218,7 +3240,7 @@
       <c r="D65" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -3243,7 +3265,7 @@
       <c r="D66" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F66" s="4" t="s">
@@ -3268,7 +3290,7 @@
       <c r="D67" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F67" s="4" t="s">
@@ -3293,7 +3315,7 @@
       <c r="D68" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -3318,7 +3340,7 @@
       <c r="D69" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -3343,7 +3365,7 @@
       <c r="D70" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F70" s="4" t="s">
@@ -3368,7 +3390,7 @@
       <c r="D71" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -3393,7 +3415,7 @@
       <c r="D72" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F72" s="4" t="s">
@@ -3418,7 +3440,7 @@
       <c r="D73" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F73" s="4" t="s">
@@ -3443,7 +3465,7 @@
       <c r="D74" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F74" s="4" t="s">
@@ -3468,7 +3490,7 @@
       <c r="D75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F75" s="4" t="s">
@@ -3493,7 +3515,7 @@
       <c r="D76" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F76" s="4" t="s">
@@ -3518,7 +3540,7 @@
       <c r="D77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F77" s="4" t="s">
@@ -3543,7 +3565,7 @@
       <c r="D78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F78" s="4" t="s">
@@ -3568,7 +3590,7 @@
       <c r="D79" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F79" s="4" t="s">
@@ -3593,7 +3615,7 @@
       <c r="D80" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F80" s="4" t="s">
@@ -3618,7 +3640,7 @@
       <c r="D81" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F81" s="4" t="s">
@@ -3643,7 +3665,7 @@
       <c r="D82" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F82" s="4" t="s">
@@ -3668,7 +3690,7 @@
       <c r="D83" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F83" s="4" t="s">
@@ -3693,7 +3715,7 @@
       <c r="D84" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F84" s="4" t="s">
@@ -3718,7 +3740,7 @@
       <c r="D85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F85" s="4" t="s">
@@ -3743,7 +3765,7 @@
       <c r="D86" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F86" s="4" t="s">
@@ -3768,7 +3790,7 @@
       <c r="D87" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F87" s="4" t="s">
@@ -3793,7 +3815,7 @@
       <c r="D88" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F88" s="4" t="s">
@@ -3818,7 +3840,7 @@
       <c r="D89" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F89" s="4" t="s">
@@ -3843,7 +3865,7 @@
       <c r="D90" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="4" t="s">
@@ -3868,7 +3890,7 @@
       <c r="D91" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E91" s="4" t="s">
+      <c r="E91" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F91" s="4" t="s">
@@ -3893,7 +3915,7 @@
       <c r="D92" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F92" s="4" t="s">
@@ -3918,7 +3940,7 @@
       <c r="D93" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="E93" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F93" s="4" t="s">
@@ -3943,7 +3965,7 @@
       <c r="D94" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E94" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F94" s="4" t="s">
@@ -3968,7 +3990,7 @@
       <c r="D95" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E95" s="4" t="s">
+      <c r="E95" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F95" s="4" t="s">
@@ -3993,7 +4015,7 @@
       <c r="D96" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F96" s="4" t="s">
@@ -4018,7 +4040,7 @@
       <c r="D97" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E97" s="4" t="s">
+      <c r="E97" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F97" s="4" t="s">
@@ -4043,7 +4065,7 @@
       <c r="D98" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E98" s="4" t="s">
+      <c r="E98" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F98" s="4" t="s">
@@ -4068,7 +4090,7 @@
       <c r="D99" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E99" s="4" t="s">
+      <c r="E99" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F99" s="4" t="s">
@@ -4093,7 +4115,7 @@
       <c r="D100" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E100" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F100" s="4" t="s">
@@ -4118,7 +4140,7 @@
       <c r="D101" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E101" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F101" s="4" t="s">
@@ -4143,7 +4165,7 @@
       <c r="D102" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F102" s="4" t="s">
@@ -4168,7 +4190,7 @@
       <c r="D103" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E103" s="4" t="s">
+      <c r="E103" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F103" s="4" t="s">
@@ -4193,7 +4215,7 @@
       <c r="D104" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E104" s="4" t="s">
+      <c r="E104" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F104" s="4" t="s">
@@ -4218,7 +4240,7 @@
       <c r="D105" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E105" s="4" t="s">
+      <c r="E105" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F105" s="4" t="s">
@@ -4243,7 +4265,7 @@
       <c r="D106" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E106" s="4" t="s">
+      <c r="E106" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F106" s="4" t="s">
@@ -4268,7 +4290,7 @@
       <c r="D107" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E107" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F107" s="4" t="s">
@@ -4293,7 +4315,7 @@
       <c r="D108" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="E108" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F108" s="4" t="s">
@@ -4318,7 +4340,7 @@
       <c r="D109" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F109" s="4" t="s">
@@ -4343,7 +4365,7 @@
       <c r="D110" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E110" s="4" t="s">
+      <c r="E110" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F110" s="4" t="s">
@@ -4368,7 +4390,7 @@
       <c r="D111" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E111" s="4" t="s">
+      <c r="E111" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F111" s="4" t="s">
@@ -4393,7 +4415,7 @@
       <c r="D112" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E112" s="4" t="s">
+      <c r="E112" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F112" s="4" t="s">
@@ -4418,7 +4440,7 @@
       <c r="D113" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E113" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F113" s="4" t="s">
@@ -4443,7 +4465,7 @@
       <c r="D114" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E114" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F114" s="4" t="s">
@@ -4468,7 +4490,7 @@
       <c r="D115" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E115" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F115" s="4" t="s">
@@ -4493,7 +4515,7 @@
       <c r="D116" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E116" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F116" s="4" t="s">
@@ -4518,7 +4540,7 @@
       <c r="D117" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E117" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F117" s="4" t="s">
@@ -4543,7 +4565,7 @@
       <c r="D118" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E118" s="4" t="s">
+      <c r="E118" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F118" s="4" t="s">
@@ -4568,7 +4590,7 @@
       <c r="D119" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E119" s="4" t="s">
+      <c r="E119" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F119" s="4" t="s">
@@ -4593,7 +4615,7 @@
       <c r="D120" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E120" s="4" t="s">
+      <c r="E120" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F120" s="4" t="s">
@@ -4618,7 +4640,7 @@
       <c r="D121" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E121" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F121" s="4" t="s">
@@ -4643,7 +4665,7 @@
       <c r="D122" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E122" s="4" t="s">
+      <c r="E122" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F122" s="4" t="s">
@@ -4668,7 +4690,7 @@
       <c r="D123" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E123" s="4" t="s">
+      <c r="E123" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F123" s="4" t="s">
@@ -4693,7 +4715,7 @@
       <c r="D124" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E124" s="4" t="s">
+      <c r="E124" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F124" s="4" t="s">
@@ -4718,7 +4740,7 @@
       <c r="D125" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E125" s="4" t="s">
+      <c r="E125" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F125" s="4" t="s">
@@ -4743,7 +4765,7 @@
       <c r="D126" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E126" s="4" t="s">
+      <c r="E126" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F126" s="4" t="s">
@@ -4768,7 +4790,7 @@
       <c r="D127" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E127" s="4" t="s">
+      <c r="E127" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F127" s="4" t="s">
@@ -4793,7 +4815,7 @@
       <c r="D128" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E128" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F128" s="4" t="s">
@@ -4818,7 +4840,7 @@
       <c r="D129" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E129" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F129" s="4" t="s">
@@ -4843,7 +4865,7 @@
       <c r="D130" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E130" s="4" t="s">
+      <c r="E130" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F130" s="4" t="s">
@@ -4868,7 +4890,7 @@
       <c r="D131" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E131" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F131" s="4" t="s">
@@ -4893,7 +4915,7 @@
       <c r="D132" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E132" s="4" t="s">
+      <c r="E132" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F132" s="4" t="s">
@@ -4918,7 +4940,7 @@
       <c r="D133" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E133" s="4" t="s">
+      <c r="E133" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F133" s="4" t="s">
@@ -4943,7 +4965,7 @@
       <c r="D134" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E134" s="4" t="s">
+      <c r="E134" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F134" s="4" t="s">
@@ -4968,7 +4990,7 @@
       <c r="D135" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E135" s="4" t="s">
+      <c r="E135" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F135" s="4" t="s">
@@ -4993,7 +5015,7 @@
       <c r="D136" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E136" s="4" t="s">
+      <c r="E136" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F136" s="4" t="s">
@@ -5018,7 +5040,7 @@
       <c r="D137" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="E137" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F137" s="4" t="s">
@@ -5043,7 +5065,7 @@
       <c r="D138" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F138" s="4" t="s">
@@ -5068,7 +5090,7 @@
       <c r="D139" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E139" s="4" t="s">
+      <c r="E139" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F139" s="4" t="s">
@@ -5093,7 +5115,7 @@
       <c r="D140" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E140" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F140" s="4" t="s">
@@ -5118,7 +5140,7 @@
       <c r="D141" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="E141" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F141" s="4" t="s">
@@ -5143,7 +5165,7 @@
       <c r="D142" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E142" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F142" s="4" t="s">
@@ -5168,7 +5190,7 @@
       <c r="D143" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E143" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F143" s="4" t="s">
@@ -5193,7 +5215,7 @@
       <c r="D144" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E144" s="4" t="s">
+      <c r="E144" s="8" t="s">
         <v>282</v>
       </c>
       <c r="F144" s="4" t="s">
@@ -5218,7 +5240,7 @@
       <c r="D145" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E145" s="4" t="s">
+      <c r="E145" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F145" s="4" t="s">
@@ -5235,7 +5257,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>62</v>
@@ -5243,11 +5265,11 @@
       <c r="D146" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E146" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G146" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F146</f>
@@ -5260,7 +5282,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>62</v>
@@ -5268,15 +5290,15 @@
       <c r="D147" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E147" s="4" t="s">
-        <v>308</v>
+      <c r="E147" s="8" t="s">
+        <v>330</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G147" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F147</f>
-        <v>taunt_action_pickup_Key</v>
+        <v>taunt_activity_pickup_Key</v>
       </c>
       <c r="H147" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5285,7 +5307,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>62</v>
@@ -5293,15 +5315,15 @@
       <c r="D148" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E148" s="4" t="s">
-        <v>311</v>
+      <c r="E148" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="G148" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F148</f>
-        <v>taunt_action_facilitytime_5Min1</v>
+        <v>taunt_activity_facilitytime_5Min1</v>
       </c>
       <c r="H148" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5310,7 +5332,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>62</v>
@@ -5318,15 +5340,15 @@
       <c r="D149" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E149" s="4" t="s">
-        <v>311</v>
+      <c r="E149" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G149" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F149</f>
-        <v>taunt_action_facilitytime_5Min2</v>
+        <v>taunt_activity_facilitytime_5Min2</v>
       </c>
       <c r="H149" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5335,7 +5357,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>62</v>
@@ -5343,15 +5365,15 @@
       <c r="D150" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E150" s="4" t="s">
-        <v>310</v>
+      <c r="E150" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G150" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F150</f>
-        <v>taunt_action_killedenemy_Gargoyle</v>
+        <v>taunt_activity_killedenemy_Gargoyle</v>
       </c>
       <c r="H150" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5360,7 +5382,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>62</v>
@@ -5368,15 +5390,15 @@
       <c r="D151" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E151" s="4" t="s">
-        <v>310</v>
+      <c r="E151" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>61</v>
+        <v>335</v>
       </c>
       <c r="G151" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F151</f>
-        <v>taunt_action_killedenemy_Bracken</v>
+        <v>taunt_activity_killedenemy_Flowerman</v>
       </c>
       <c r="H151" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5385,7 +5407,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>62</v>
@@ -5393,15 +5415,15 @@
       <c r="D152" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E152" s="4" t="s">
-        <v>310</v>
+      <c r="E152" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>296</v>
       </c>
       <c r="G152" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F152</f>
-        <v>taunt_action_killedenemy_Butler</v>
+        <v>taunt_activity_killedenemy_Butler</v>
       </c>
       <c r="H152" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5410,7 +5432,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>62</v>
@@ -5418,15 +5440,15 @@
       <c r="D153" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E153" s="4" t="s">
-        <v>310</v>
+      <c r="E153" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F153" s="4" t="s">
         <v>297</v>
       </c>
       <c r="G153" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F153</f>
-        <v>taunt_action_killedenemy_Centipede</v>
+        <v>taunt_activity_killedenemy_Centipede</v>
       </c>
       <c r="H153" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5435,7 +5457,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>62</v>
@@ -5443,15 +5465,15 @@
       <c r="D154" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E154" s="4" t="s">
-        <v>310</v>
+      <c r="E154" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="G154" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F154</f>
-        <v>taunt_action_killedenemy_GhostGirl</v>
+        <v>taunt_activity_killedenemy_Girl</v>
       </c>
       <c r="H154" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5460,7 +5482,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>62</v>
@@ -5468,15 +5490,15 @@
       <c r="D155" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E155" s="4" t="s">
-        <v>310</v>
+      <c r="E155" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
       <c r="G155" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F155</f>
-        <v>taunt_action_killedenemy_HoardingBug</v>
+        <v>taunt_activity_killedenemy_Hoarding Bug</v>
       </c>
       <c r="H155" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5485,7 +5507,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>62</v>
@@ -5493,15 +5515,15 @@
       <c r="D156" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E156" s="4" t="s">
-        <v>310</v>
+      <c r="E156" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G156" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F156</f>
-        <v>taunt_action_killedenemy_Jester</v>
+        <v>taunt_activity_killedenemy_Jester</v>
       </c>
       <c r="H156" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5510,7 +5532,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>62</v>
@@ -5518,15 +5540,15 @@
       <c r="D157" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E157" s="4" t="s">
-        <v>310</v>
+      <c r="E157" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G157" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F157</f>
-        <v>taunt_action_killedenemy_Maneater</v>
+        <v>taunt_activity_killedenemy_Maneater</v>
       </c>
       <c r="H157" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5535,7 +5557,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>62</v>
@@ -5543,15 +5565,15 @@
       <c r="D158" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E158" s="4" t="s">
-        <v>310</v>
+      <c r="E158" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G158" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F158</f>
-        <v>taunt_action_killedenemy_Masked</v>
+        <v>taunt_activity_killedenemy_Masked</v>
       </c>
       <c r="H158" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5560,7 +5582,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>62</v>
@@ -5568,15 +5590,15 @@
       <c r="D159" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E159" s="4" t="s">
-        <v>310</v>
+      <c r="E159" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F159" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G159" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F159</f>
-        <v>taunt_action_killedenemy_Nutcracker</v>
+        <v>taunt_activity_killedenemy_Nutcracker</v>
       </c>
       <c r="H159" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5585,7 +5607,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>62</v>
@@ -5593,15 +5615,15 @@
       <c r="D160" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E160" s="4" t="s">
-        <v>310</v>
+      <c r="E160" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="G160" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F160</f>
-        <v>taunt_action_killedenemy_Slime</v>
+        <v>taunt_activity_killedenemy_Blob</v>
       </c>
       <c r="H160" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5610,7 +5632,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>62</v>
@@ -5618,15 +5640,15 @@
       <c r="D161" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E161" s="4" t="s">
-        <v>310</v>
+      <c r="E161" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="G161" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F161</f>
-        <v>taunt_action_killedenemy_Spider</v>
+        <v>taunt_activity_killedenemy_Bunker Spider</v>
       </c>
       <c r="H161" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5635,7 +5657,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>62</v>
@@ -5643,15 +5665,15 @@
       <c r="D162" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E162" s="4" t="s">
-        <v>310</v>
+      <c r="E162" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F162" s="4" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="G162" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F162</f>
-        <v>taunt_action_killedenemy_SpringHead</v>
+        <v>taunt_activity_killedenemy_Spring</v>
       </c>
       <c r="H162" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5660,7 +5682,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>62</v>
@@ -5668,15 +5690,15 @@
       <c r="D163" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E163" s="4" t="s">
-        <v>310</v>
+      <c r="E163" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="G163" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F163</f>
-        <v>taunt_action_killedenemy_Thumper</v>
+        <v>taunt_activity_killedenemy_Crawler</v>
       </c>
       <c r="H163" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5685,7 +5707,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>62</v>
@@ -5693,15 +5715,15 @@
       <c r="D164" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E164" s="4" t="s">
-        <v>308</v>
+      <c r="E164" s="8" t="s">
+        <v>330</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="G164" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F164</f>
-        <v>taunt_action_pickup_Apparatus</v>
+        <v>taunt_activity_pickup_Apparatus</v>
       </c>
       <c r="H164" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5710,7 +5732,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>62</v>
@@ -5718,15 +5740,15 @@
       <c r="D165" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E165" s="4" t="s">
-        <v>308</v>
+      <c r="E165" s="8" t="s">
+        <v>330</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="G165" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F165</f>
-        <v>taunt_action_pickup_Comedy</v>
+        <v>taunt_activity_pickup_Comedy</v>
       </c>
       <c r="H165" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -5735,7 +5757,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>62</v>
@@ -5743,27 +5765,52 @@
       <c r="D166" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E166" s="4" t="s">
-        <v>308</v>
+      <c r="E166" s="8" t="s">
+        <v>330</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G166" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F166</f>
-        <v>taunt_action_pickup_Tragedy</v>
+        <v>taunt_activity_pickup_Tragedy</v>
       </c>
       <c r="H166" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"Would be a tragedy if you didn't put that mask on and kill all yer friends. Hahahaha!"&lt;/pre&gt;</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G167" s="7" t="str">
+        <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F167</f>
+        <v>taunt_76561198155447311_MyCreator</v>
+      </c>
+      <c r="H167" s="7" t="str">
+        <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
+        <v>&lt;pre&gt;"If it isn't my creator! There's something I've always wanted to say to you, YOU SUCK! Hahahaha!"&lt;/pre&gt;</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat(gargoyle): Introduce gargoyle statue scrap and update assets (v0.6.0)
This commit introduces a new gargoyle statue scrap item and updates various assets for improved visuals and sound effects.

The following changes were made:

- Added new binary files for user interface elements and sound effects.
- Updated project version to 0.6.0.
- Added configuration options for statue scrap.
- Introduced `LethalGargoylesSFX` class for step sound effects.
- Added methods to clear player data in `LethalGargoylesAI`.
- Registered statue scrap and loaded sound assets.
- Updated binary files and manifests.
- Modified animation files to incorporate step sound effects.
- Added new sound effects and metadata files.
- Updated animator controller and prefab files with new components and adjustments.
- Added new assets: `GargoyleIcon.png`, `GargoyleScrap.asset`, and `GargoyleStatue.prefab`.
- Updated the main Unity scene with new components and prefab instances.
</commit_message>
<xml_diff>
--- a/AssetSources/Audio/VoiceLines.xlsx
+++ b/AssetSources/Audio/VoiceLines.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F6763-6314-4A2E-A23B-C5B22BFC094B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A02B463-AC80-43DA-BEE2-B48328E430BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="660" windowWidth="29010" windowHeight="15345" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="30105" windowHeight="20985" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Taunts" sheetId="1" r:id="rId1"/>
+    <sheet name="Personal Taunts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="367">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -1111,6 +1112,78 @@
   </si>
   <si>
     <t>MyCreator</t>
+  </si>
+  <si>
+    <t>76561198160388528</t>
+  </si>
+  <si>
+    <t>Conor_1</t>
+  </si>
+  <si>
+    <t>76561198246596240</t>
+  </si>
+  <si>
+    <t>Richard_1</t>
+  </si>
+  <si>
+    <t>76561198089920267</t>
+  </si>
+  <si>
+    <t>Caity_1</t>
+  </si>
+  <si>
+    <t>76561198145787492</t>
+  </si>
+  <si>
+    <t>Kyle_1</t>
+  </si>
+  <si>
+    <t>76561199745295802</t>
+  </si>
+  <si>
+    <t>76561199524823720</t>
+  </si>
+  <si>
+    <t>Kenai_1</t>
+  </si>
+  <si>
+    <t>Jensen_1</t>
+  </si>
+  <si>
+    <t>76561198977061815</t>
+  </si>
+  <si>
+    <t>Jace_1</t>
+  </si>
+  <si>
+    <t>76561198036923975</t>
+  </si>
+  <si>
+    <t>Zach_1</t>
+  </si>
+  <si>
+    <t>"Oi, Conor. Your friends are waiting for you at the bottom of the nearest pit. Jump down and have a look! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"Richard! I fart in yer general direction! *Fart noise*"</t>
+  </si>
+  <si>
+    <t>"Damn Caity, you look sexy. Come over here and let me give you a big… push into the nearest pit! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"It's Kyle! The biggest weeb I know."</t>
+  </si>
+  <si>
+    <t>"I'm coming to kick your butt, Jensen!"</t>
+  </si>
+  <si>
+    <t>"I'm gonna chop your legs off, Jace!"</t>
+  </si>
+  <si>
+    <t>"Better watch out, Kenai. I eat humans for breakfast!"</t>
+  </si>
+  <si>
+    <t>"Zach! I have one thing to say to you. Yer a bitch! Hahahaha!"</t>
   </si>
 </sst>
 </file>
@@ -1182,29 +1255,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="23">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1225,8 +1302,63 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1273,23 +1405,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H167" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H167" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:H167" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H139">
     <sortCondition ref="G1:G139"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{6266219D-B50E-4703-B88B-14976C41CFC3}" name="Redo" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{6266219D-B50E-4703-B88B-14976C41CFC3}" name="Redo" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="14">
       <calculatedColumnFormula>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="13">
       <calculatedColumnFormula>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0A87C6E0-96BC-49E1-80A2-745344D50B24}" name="Table14" displayName="Table14" ref="A1:G9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:G9" xr:uid="{0A87C6E0-96BC-49E1-80A2-745344D50B24}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1">
+    <sortCondition ref="G1"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CBAB328E-B65F-45C6-9BBC-E597CEE9BED7}" name="Quote" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{32DA339A-9866-4E0F-AF64-F3727485FE9C}" name="Completed?" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{C8C76300-B409-4EED-A92F-A27B5FD4E310}" name="Redo" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5EBA510C-CCAB-462E-A5AA-3C66C9899FF9}" name="Source" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{54E93EB9-CFBB-4C65-B7C0-4A7CB75216E8}" name="Type" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{FBC6144B-F744-48B4-B6DF-DC991CA90882}" name="File Name" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{495701F6-B9B2-498F-A29C-38CA360231AB}" name="Full file name" dataDxfId="4">
+      <calculatedColumnFormula>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1616,8 +1769,8 @@
   <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H167" sqref="H167"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1779,7 @@
     <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="89.42578125" customWidth="1"/>
@@ -1645,7 +1798,7 @@
       <c r="D1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1668,7 +1821,7 @@
       <c r="D2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>330</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1693,7 +1846,7 @@
       <c r="D3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1718,7 +1871,7 @@
       <c r="D4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1743,7 +1896,7 @@
       <c r="D5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1768,7 +1921,7 @@
       <c r="D6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1793,7 +1946,7 @@
       <c r="D7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1815,7 +1968,7 @@
       <c r="D8" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1840,7 +1993,7 @@
       <c r="D9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1865,7 +2018,7 @@
       <c r="D10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1890,7 +2043,7 @@
       <c r="D11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1915,7 +2068,7 @@
       <c r="D12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1940,7 +2093,7 @@
       <c r="D13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1965,7 +2118,7 @@
       <c r="D14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1990,7 +2143,7 @@
       <c r="D15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -2015,7 +2168,7 @@
       <c r="D16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -2040,7 +2193,7 @@
       <c r="D17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -2065,7 +2218,7 @@
       <c r="D18" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -2090,7 +2243,7 @@
       <c r="D19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -2115,7 +2268,7 @@
       <c r="D20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -2140,7 +2293,7 @@
       <c r="D21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -2165,7 +2318,7 @@
       <c r="D22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -2190,7 +2343,7 @@
       <c r="D23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -2215,7 +2368,7 @@
       <c r="D24" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -2240,7 +2393,7 @@
       <c r="D25" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2265,7 +2418,7 @@
       <c r="D26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -2290,7 +2443,7 @@
       <c r="D27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -2315,7 +2468,7 @@
       <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -2340,7 +2493,7 @@
       <c r="D29" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -2365,7 +2518,7 @@
       <c r="D30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F30" s="4" t="s">
@@ -2390,7 +2543,7 @@
       <c r="D31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -2415,7 +2568,7 @@
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -2440,7 +2593,7 @@
       <c r="D33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F33" s="4" t="s">
@@ -2465,7 +2618,7 @@
       <c r="D34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F34" s="4" t="s">
@@ -2490,7 +2643,7 @@
       <c r="D35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -2515,7 +2668,7 @@
       <c r="D36" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -2540,7 +2693,7 @@
       <c r="D37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F37" s="4" t="s">
@@ -2565,7 +2718,7 @@
       <c r="D38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -2590,7 +2743,7 @@
       <c r="D39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -2615,7 +2768,7 @@
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -2640,7 +2793,7 @@
       <c r="D41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F41" s="4" t="s">
@@ -2665,7 +2818,7 @@
       <c r="D42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F42" s="4" t="s">
@@ -2690,7 +2843,7 @@
       <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -2715,7 +2868,7 @@
       <c r="D44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -2740,7 +2893,7 @@
       <c r="D45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F45" s="4" t="s">
@@ -2765,7 +2918,7 @@
       <c r="D46" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F46" s="4" t="s">
@@ -2790,7 +2943,7 @@
       <c r="D47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -2815,7 +2968,7 @@
       <c r="D48" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -2840,7 +2993,7 @@
       <c r="D49" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F49" s="4" t="s">
@@ -2865,7 +3018,7 @@
       <c r="D50" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F50" s="4" t="s">
@@ -2890,7 +3043,7 @@
       <c r="D51" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F51" s="4" t="s">
@@ -2915,7 +3068,7 @@
       <c r="D52" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F52" s="4" t="s">
@@ -2940,7 +3093,7 @@
       <c r="D53" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F53" s="4" t="s">
@@ -2965,7 +3118,7 @@
       <c r="D54" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F54" s="4" t="s">
@@ -2990,7 +3143,7 @@
       <c r="D55" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F55" s="4" t="s">
@@ -3015,7 +3168,7 @@
       <c r="D56" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -3040,7 +3193,7 @@
       <c r="D57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -3065,7 +3218,7 @@
       <c r="D58" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F58" s="4" t="s">
@@ -3090,7 +3243,7 @@
       <c r="D59" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="7" t="s">
         <v>85</v>
       </c>
       <c r="F59" s="4" t="s">
@@ -3115,7 +3268,7 @@
       <c r="D60" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="7" t="s">
         <v>85</v>
       </c>
       <c r="F60" s="4" t="s">
@@ -3140,7 +3293,7 @@
       <c r="D61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E61" s="7" t="s">
         <v>85</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -3165,7 +3318,7 @@
       <c r="D62" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -3190,7 +3343,7 @@
       <c r="D63" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F63" s="4" t="s">
@@ -3215,7 +3368,7 @@
       <c r="D64" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -3240,7 +3393,7 @@
       <c r="D65" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -3265,7 +3418,7 @@
       <c r="D66" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F66" s="4" t="s">
@@ -3290,7 +3443,7 @@
       <c r="D67" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E67" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F67" s="4" t="s">
@@ -3315,7 +3468,7 @@
       <c r="D68" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -3340,7 +3493,7 @@
       <c r="D69" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -3365,7 +3518,7 @@
       <c r="D70" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E70" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F70" s="4" t="s">
@@ -3390,7 +3543,7 @@
       <c r="D71" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -3415,7 +3568,7 @@
       <c r="D72" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E72" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F72" s="4" t="s">
@@ -3440,7 +3593,7 @@
       <c r="D73" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F73" s="4" t="s">
@@ -3465,7 +3618,7 @@
       <c r="D74" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F74" s="4" t="s">
@@ -3490,7 +3643,7 @@
       <c r="D75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F75" s="4" t="s">
@@ -3515,7 +3668,7 @@
       <c r="D76" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F76" s="4" t="s">
@@ -3540,7 +3693,7 @@
       <c r="D77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E77" s="8" t="s">
+      <c r="E77" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F77" s="4" t="s">
@@ -3565,7 +3718,7 @@
       <c r="D78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F78" s="4" t="s">
@@ -3590,7 +3743,7 @@
       <c r="D79" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E79" s="8" t="s">
+      <c r="E79" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F79" s="4" t="s">
@@ -3615,7 +3768,7 @@
       <c r="D80" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E80" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F80" s="4" t="s">
@@ -3640,7 +3793,7 @@
       <c r="D81" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E81" s="8" t="s">
+      <c r="E81" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F81" s="4" t="s">
@@ -3665,7 +3818,7 @@
       <c r="D82" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="E82" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F82" s="4" t="s">
@@ -3690,7 +3843,7 @@
       <c r="D83" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E83" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F83" s="4" t="s">
@@ -3715,7 +3868,7 @@
       <c r="D84" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F84" s="4" t="s">
@@ -3740,7 +3893,7 @@
       <c r="D85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E85" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F85" s="4" t="s">
@@ -3765,7 +3918,7 @@
       <c r="D86" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="E86" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F86" s="4" t="s">
@@ -3790,7 +3943,7 @@
       <c r="D87" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F87" s="4" t="s">
@@ -3815,7 +3968,7 @@
       <c r="D88" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F88" s="4" t="s">
@@ -3840,7 +3993,7 @@
       <c r="D89" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F89" s="4" t="s">
@@ -3865,7 +4018,7 @@
       <c r="D90" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="4" t="s">
@@ -3890,7 +4043,7 @@
       <c r="D91" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F91" s="4" t="s">
@@ -3915,7 +4068,7 @@
       <c r="D92" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F92" s="4" t="s">
@@ -3940,7 +4093,7 @@
       <c r="D93" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E93" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F93" s="4" t="s">
@@ -3965,7 +4118,7 @@
       <c r="D94" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="E94" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F94" s="4" t="s">
@@ -3990,7 +4143,7 @@
       <c r="D95" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F95" s="4" t="s">
@@ -4015,7 +4168,7 @@
       <c r="D96" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E96" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F96" s="4" t="s">
@@ -4040,7 +4193,7 @@
       <c r="D97" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E97" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F97" s="4" t="s">
@@ -4065,7 +4218,7 @@
       <c r="D98" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="E98" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F98" s="4" t="s">
@@ -4090,7 +4243,7 @@
       <c r="D99" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E99" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F99" s="4" t="s">
@@ -4115,7 +4268,7 @@
       <c r="D100" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F100" s="4" t="s">
@@ -4140,7 +4293,7 @@
       <c r="D101" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E101" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F101" s="4" t="s">
@@ -4165,7 +4318,7 @@
       <c r="D102" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E102" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F102" s="4" t="s">
@@ -4190,7 +4343,7 @@
       <c r="D103" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E103" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F103" s="4" t="s">
@@ -4215,7 +4368,7 @@
       <c r="D104" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E104" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F104" s="4" t="s">
@@ -4240,7 +4393,7 @@
       <c r="D105" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F105" s="4" t="s">
@@ -4265,7 +4418,7 @@
       <c r="D106" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E106" s="8" t="s">
+      <c r="E106" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F106" s="4" t="s">
@@ -4290,7 +4443,7 @@
       <c r="D107" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E107" s="8" t="s">
+      <c r="E107" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F107" s="4" t="s">
@@ -4315,7 +4468,7 @@
       <c r="D108" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E108" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F108" s="4" t="s">
@@ -4340,7 +4493,7 @@
       <c r="D109" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E109" s="8" t="s">
+      <c r="E109" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F109" s="4" t="s">
@@ -4365,7 +4518,7 @@
       <c r="D110" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="E110" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F110" s="4" t="s">
@@ -4390,7 +4543,7 @@
       <c r="D111" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="E111" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F111" s="4" t="s">
@@ -4415,7 +4568,7 @@
       <c r="D112" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E112" s="8" t="s">
+      <c r="E112" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F112" s="4" t="s">
@@ -4440,7 +4593,7 @@
       <c r="D113" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E113" s="8" t="s">
+      <c r="E113" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F113" s="4" t="s">
@@ -4465,7 +4618,7 @@
       <c r="D114" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E114" s="8" t="s">
+      <c r="E114" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F114" s="4" t="s">
@@ -4490,7 +4643,7 @@
       <c r="D115" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E115" s="8" t="s">
+      <c r="E115" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F115" s="4" t="s">
@@ -4515,7 +4668,7 @@
       <c r="D116" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E116" s="8" t="s">
+      <c r="E116" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F116" s="4" t="s">
@@ -4540,7 +4693,7 @@
       <c r="D117" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E117" s="8" t="s">
+      <c r="E117" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F117" s="4" t="s">
@@ -4565,7 +4718,7 @@
       <c r="D118" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E118" s="8" t="s">
+      <c r="E118" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F118" s="4" t="s">
@@ -4590,7 +4743,7 @@
       <c r="D119" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E119" s="8" t="s">
+      <c r="E119" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F119" s="4" t="s">
@@ -4615,7 +4768,7 @@
       <c r="D120" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E120" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F120" s="4" t="s">
@@ -4640,7 +4793,7 @@
       <c r="D121" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E121" s="8" t="s">
+      <c r="E121" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F121" s="4" t="s">
@@ -4665,7 +4818,7 @@
       <c r="D122" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E122" s="8" t="s">
+      <c r="E122" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F122" s="4" t="s">
@@ -4690,7 +4843,7 @@
       <c r="D123" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E123" s="8" t="s">
+      <c r="E123" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F123" s="4" t="s">
@@ -4715,7 +4868,7 @@
       <c r="D124" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E124" s="8" t="s">
+      <c r="E124" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F124" s="4" t="s">
@@ -4740,7 +4893,7 @@
       <c r="D125" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E125" s="8" t="s">
+      <c r="E125" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F125" s="4" t="s">
@@ -4765,7 +4918,7 @@
       <c r="D126" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="E126" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F126" s="4" t="s">
@@ -4790,7 +4943,7 @@
       <c r="D127" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E127" s="8" t="s">
+      <c r="E127" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F127" s="4" t="s">
@@ -4815,7 +4968,7 @@
       <c r="D128" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="E128" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F128" s="4" t="s">
@@ -4840,7 +4993,7 @@
       <c r="D129" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E129" s="8" t="s">
+      <c r="E129" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F129" s="4" t="s">
@@ -4865,7 +5018,7 @@
       <c r="D130" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E130" s="8" t="s">
+      <c r="E130" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F130" s="4" t="s">
@@ -4890,7 +5043,7 @@
       <c r="D131" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E131" s="8" t="s">
+      <c r="E131" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F131" s="4" t="s">
@@ -4915,7 +5068,7 @@
       <c r="D132" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E132" s="8" t="s">
+      <c r="E132" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F132" s="4" t="s">
@@ -4940,7 +5093,7 @@
       <c r="D133" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="E133" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F133" s="4" t="s">
@@ -4965,7 +5118,7 @@
       <c r="D134" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E134" s="8" t="s">
+      <c r="E134" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F134" s="4" t="s">
@@ -4990,7 +5143,7 @@
       <c r="D135" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E135" s="8" t="s">
+      <c r="E135" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F135" s="4" t="s">
@@ -5015,7 +5168,7 @@
       <c r="D136" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E136" s="8" t="s">
+      <c r="E136" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F136" s="4" t="s">
@@ -5040,7 +5193,7 @@
       <c r="D137" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E137" s="8" t="s">
+      <c r="E137" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F137" s="4" t="s">
@@ -5065,7 +5218,7 @@
       <c r="D138" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E138" s="8" t="s">
+      <c r="E138" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F138" s="4" t="s">
@@ -5090,7 +5243,7 @@
       <c r="D139" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E139" s="8" t="s">
+      <c r="E139" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F139" s="4" t="s">
@@ -5115,7 +5268,7 @@
       <c r="D140" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E140" s="8" t="s">
+      <c r="E140" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F140" s="4" t="s">
@@ -5140,7 +5293,7 @@
       <c r="D141" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E141" s="8" t="s">
+      <c r="E141" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F141" s="4" t="s">
@@ -5165,7 +5318,7 @@
       <c r="D142" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F142" s="4" t="s">
@@ -5190,7 +5343,7 @@
       <c r="D143" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E143" s="8" t="s">
+      <c r="E143" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F143" s="4" t="s">
@@ -5215,7 +5368,7 @@
       <c r="D144" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E144" s="8" t="s">
+      <c r="E144" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F144" s="4" t="s">
@@ -5240,7 +5393,7 @@
       <c r="D145" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E145" s="8" t="s">
+      <c r="E145" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F145" s="4" t="s">
@@ -5265,7 +5418,7 @@
       <c r="D146" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E146" s="8" t="s">
+      <c r="E146" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F146" s="4" t="s">
@@ -5290,7 +5443,7 @@
       <c r="D147" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E147" s="8" t="s">
+      <c r="E147" s="7" t="s">
         <v>330</v>
       </c>
       <c r="F147" s="4" t="s">
@@ -5315,7 +5468,7 @@
       <c r="D148" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E148" s="8" t="s">
+      <c r="E148" s="7" t="s">
         <v>332</v>
       </c>
       <c r="F148" s="4" t="s">
@@ -5340,7 +5493,7 @@
       <c r="D149" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E149" s="8" t="s">
+      <c r="E149" s="7" t="s">
         <v>332</v>
       </c>
       <c r="F149" s="4" t="s">
@@ -5365,7 +5518,7 @@
       <c r="D150" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E150" s="8" t="s">
+      <c r="E150" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F150" s="4" t="s">
@@ -5390,7 +5543,7 @@
       <c r="D151" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E151" s="8" t="s">
+      <c r="E151" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F151" s="4" t="s">
@@ -5415,7 +5568,7 @@
       <c r="D152" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E152" s="8" t="s">
+      <c r="E152" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F152" s="4" t="s">
@@ -5440,7 +5593,7 @@
       <c r="D153" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E153" s="8" t="s">
+      <c r="E153" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F153" s="4" t="s">
@@ -5465,7 +5618,7 @@
       <c r="D154" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E154" s="8" t="s">
+      <c r="E154" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F154" s="4" t="s">
@@ -5490,7 +5643,7 @@
       <c r="D155" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E155" s="8" t="s">
+      <c r="E155" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F155" s="4" t="s">
@@ -5515,7 +5668,7 @@
       <c r="D156" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E156" s="8" t="s">
+      <c r="E156" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F156" s="4" t="s">
@@ -5540,7 +5693,7 @@
       <c r="D157" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E157" s="8" t="s">
+      <c r="E157" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F157" s="4" t="s">
@@ -5565,7 +5718,7 @@
       <c r="D158" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E158" s="8" t="s">
+      <c r="E158" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F158" s="4" t="s">
@@ -5590,7 +5743,7 @@
       <c r="D159" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E159" s="8" t="s">
+      <c r="E159" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F159" s="4" t="s">
@@ -5615,7 +5768,7 @@
       <c r="D160" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E160" s="8" t="s">
+      <c r="E160" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F160" s="4" t="s">
@@ -5640,7 +5793,7 @@
       <c r="D161" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E161" s="8" t="s">
+      <c r="E161" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F161" s="4" t="s">
@@ -5665,7 +5818,7 @@
       <c r="D162" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E162" s="8" t="s">
+      <c r="E162" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F162" s="4" t="s">
@@ -5690,7 +5843,7 @@
       <c r="D163" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E163" s="8" t="s">
+      <c r="E163" s="7" t="s">
         <v>331</v>
       </c>
       <c r="F163" s="4" t="s">
@@ -5715,7 +5868,7 @@
       <c r="D164" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E164" s="8" t="s">
+      <c r="E164" s="7" t="s">
         <v>330</v>
       </c>
       <c r="F164" s="4" t="s">
@@ -5740,7 +5893,7 @@
       <c r="D165" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="E165" s="7" t="s">
         <v>330</v>
       </c>
       <c r="F165" s="4" t="s">
@@ -5765,7 +5918,7 @@
       <c r="D166" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E166" s="8" t="s">
+      <c r="E166" s="7" t="s">
         <v>330</v>
       </c>
       <c r="F166" s="4" t="s">
@@ -5790,27 +5943,27 @@
       <c r="D167" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E167" s="8" t="s">
+      <c r="E167" s="7" t="s">
         <v>341</v>
       </c>
       <c r="F167" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="G167" s="7" t="str">
+      <c r="G167" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F167</f>
         <v>taunt_76561198155447311_MyCreator</v>
       </c>
-      <c r="H167" s="7" t="str">
+      <c r="H167" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"If it isn't my creator! There's something I've always wanted to say to you, YOU SUCK! Hahahaha!"&lt;/pre&gt;</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5820,4 +5973,230 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFBA499-6148-4057-B788-BD118DB2B3C0}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="129.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G2" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F2</f>
+        <v>76561198160388528_Conor_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G3" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F3</f>
+        <v>76561198246596240_Richard_1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F4</f>
+        <v>76561198089920267_Caity_1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F5</f>
+        <v>76561198145787492_Kyle_1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G6" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F6</f>
+        <v>76561199745295802_Kenai_1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="G7" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F7</f>
+        <v>76561199524823720_Jensen_1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="G8" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F8</f>
+        <v>76561198977061815_Jace_1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="G9" s="9" t="str">
+        <f>IF(LEFT(Table14[[#This Row],[Type]],4)="7656","","taunt_") &amp; LOWER(Table14[[#This Row],[Type]]) &amp; "_" &amp; F9</f>
+        <v>76561198036923975_Zach_1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>